<commit_message>
Finalizazione fase2 per domani
</commit_message>
<xml_diff>
--- a/02-Schede/NT_cost_efficiency_Cronometer.xlsx
+++ b/02-Schede/NT_cost_efficiency_Cronometer.xlsx
@@ -295,72 +295,76 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,402 +613,402 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="16.9" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="5.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <f aca="false">1.99/0.5*B2/1000</f>
         <v>0.5572</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <f aca="false">IF(D2&gt;0, E2/D2, 0)</f>
         <v>5.3840631730079</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="n">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <f aca="false">7.23*B3/1000</f>
         <v>0.11568</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <f aca="false">IF(D3&gt;0, E3/D3, 0)</f>
         <v>8.64453665283541</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <f aca="false">650</f>
         <v>650</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <f aca="false">(4+0.5)/2.46*B4/1000</f>
         <v>1.1890243902439</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <f aca="false">IF(D4&gt;0, E4/D4, 0)</f>
         <v>5.04615384615385</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="n">
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <f aca="false">1.89*B5/1000</f>
         <v>0.4725</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <f aca="false">IF(D5&gt;0, E5/D5, 0)</f>
         <v>4.23280423280423</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="n">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <f aca="false">1.29/0.7*B6/1000</f>
         <v>0.921428571428572</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <f aca="false">IF(D6&gt;0, E6/D6, 0)</f>
         <v>3.25581395348837</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="n">
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <f aca="false">2.19/0.5*B7/1000</f>
         <v>2.19</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <f aca="false">IF(D7&gt;0, E7/D7, 0)</f>
         <v>2.73972602739726</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <f aca="false">(5*2+2)/7</f>
         <v>1.71428571428571</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <f aca="false">0.99*B8</f>
         <v>1.69714285714286</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <f aca="false">IF(D8&gt;0, E8/D8, 0)</f>
         <v>1.17845117845118</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3" t="n">
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4" t="n">
         <f aca="false">17.9*B9/1000</f>
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="4" t="n">
         <f aca="false">IF(D9&gt;0, E9/D9, 0)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="4" t="n">
         <f aca="false">2/20*B10</f>
         <v>0.1</v>
       </c>
-      <c r="E10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="n">
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="n">
         <f aca="false">IF(D10&gt;0, E10/D10, 0)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="n">
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="n">
         <f aca="false">20.99*B11/1000</f>
         <v>0.08396</v>
       </c>
-      <c r="E11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="n">
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="n">
         <f aca="false">IF(D11&gt;0, E11/D11, 0)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="G11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="3" t="n">
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <f aca="false">31.44*B12/1000</f>
         <v>0.6288</v>
       </c>
-      <c r="E12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="3" t="n">
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="n">
         <f aca="false">IF(D12&gt;0, E12/D12, 0)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="G12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="n">
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="n">
         <f aca="false">34.95/3*B13/1000</f>
         <v>0.699</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3" t="n">
+      <c r="E13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="n">
         <f aca="false">IF(D13&gt;0, E13/D13, 0)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="0" t="s">
+      <c r="G13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5" t="n">
+      <c r="B14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="6" t="n">
         <f aca="false">11*B14/1000</f>
         <v>0</v>
       </c>
-      <c r="E14" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="5" t="n">
+      <c r="E14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6" t="n">
         <f aca="false">IF(D14&gt;0, E14/D14, 0)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="0" t="s">
+      <c r="G14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8" t="n">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9" t="n">
         <f aca="false">SUM(D2:D14)</f>
         <v>8.65473581881533</v>
       </c>
-      <c r="E15" s="9" t="n">
+      <c r="E15" s="10" t="n">
         <f aca="false">SUM(E2:E14)</f>
         <v>24</v>
       </c>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="9" t="n">
         <f aca="false">IF(D15&gt;0, E15/D15, 0)</f>
         <v>2.7730482480845</v>
       </c>
@@ -1034,352 +1038,352 @@
   <dimension ref="A1:H1048573"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <f aca="false">1.99/0.5*B2/1000</f>
         <v>0.5572</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <f aca="false">IF(D2&gt;0, E2/D2, 0)</f>
         <v>7.17875089734386</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="n">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <f aca="false">7.23*B3/1000</f>
         <v>0.11568</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <f aca="false">IF(D3&gt;0, E3/D3, 0)</f>
         <v>8.64453665283541</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>700</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <f aca="false">(4+0.5)/2.46*B4/1000</f>
         <v>1.28048780487805</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <f aca="false">IF(D4&gt;0, E4/D4, 0)</f>
         <v>4.68571428571429</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="n">
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <f aca="false">1.89*B5/1000</f>
         <v>0.4725</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <f aca="false">IF(D5&gt;0, E5/D5, 0)</f>
         <v>4.23280423280423</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="n">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <f aca="false">2.19/0.5*B6/1000</f>
         <v>2.19</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <f aca="false">IF(D6&gt;0, E6/D6, 0)</f>
         <v>3.65296803652968</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="n">
+      <c r="B7" s="1" t="n">
+        <v>750</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <f aca="false">1.29/0.7*B7/1000</f>
-        <v>1.47428571428571</v>
-      </c>
-      <c r="E7" s="1" t="n">
+        <v>1.38214285714286</v>
+      </c>
+      <c r="E7" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <f aca="false">IF(D7&gt;0, E7/D7, 0)</f>
-        <v>2.03488372093023</v>
-      </c>
-      <c r="G7" s="0" t="s">
+        <v>2.17054263565891</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="n">
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="n">
         <f aca="false">17.9*B8/1000</f>
         <v>0</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <f aca="false">IF(D8&gt;0, E8/D8, 0)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <f aca="false">2/20*B9</f>
         <v>0.1</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="n">
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="n">
         <f aca="false">IF(D9&gt;0, E9/D9, 0)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="n">
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="n">
         <f aca="false">20.99*B10/1000</f>
         <v>0.08396</v>
       </c>
-      <c r="E10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="n">
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="n">
         <f aca="false">IF(D10&gt;0, E10/D10, 0)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="0" t="s">
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="5" t="n">
         <f aca="false">(5*2+2)/7</f>
         <v>1.71428571428571</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="4" t="n">
         <f aca="false">0.99*B11</f>
         <v>1.69714285714286</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="4" t="n">
         <f aca="false">IF(D11&gt;0, E11/D11, 0)</f>
         <v>1.17845117845118</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="3" t="n">
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <f aca="false">11*B12/1000</f>
         <v>0.044</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="4" t="n">
         <f aca="false">IF(D12&gt;0, E12/D12, 0)</f>
         <v>22.7272727272727</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="G12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="10" t="n">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="11" t="n">
         <f aca="false">SUM(D2:D12)</f>
-        <v>8.01525637630662</v>
-      </c>
-      <c r="E13" s="11" t="n">
+        <v>7.92311351916377</v>
+      </c>
+      <c r="E13" s="12" t="n">
         <f aca="false">SUM(E2:E12)</f>
         <v>28</v>
       </c>
-      <c r="F13" s="10" t="n">
+      <c r="F13" s="11" t="n">
         <f aca="false">IF(D13&gt;0, E13/D13, 0)</f>
-        <v>3.49333804003687</v>
+        <v>3.53396425941342</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1414,321 +1418,321 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <f aca="false">1.99/0.5*B2/1000</f>
         <v>0.5572</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <f aca="false">IF(D2&gt;0, E2/D2, 0)</f>
         <v>7.17875089734386</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="n">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <f aca="false">17.9*B3/1000</f>
         <v>0.0716</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <f aca="false">IF(D3&gt;0, E3/D3, 0)</f>
         <v>13.9664804469274</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <f aca="false">20.99*B4/1000</f>
         <v>0.08396</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <f aca="false">IF(D4&gt;0, E4/D4, 0)</f>
         <v>11.9104335397808</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="n">
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <f aca="false">(4+0.5)/2.46*B5/1000</f>
         <v>1.09756097560976</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <f aca="false">IF(D5&gt;0, E5/D5, 0)</f>
         <v>7.28888888888889</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="n">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <f aca="false">1.89*B6/1000</f>
         <v>0.4725</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <f aca="false">IF(D6&gt;0, E6/D6, 0)</f>
         <v>4.23280423280423</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="n">
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <f aca="false">2.19/0.5*B7/1000</f>
         <v>2.19</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <f aca="false">IF(D7&gt;0, E7/D7, 0)</f>
         <v>3.65296803652968</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="n">
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="n">
         <f aca="false">1.29/0.7*B8/1000</f>
         <v>1.84285714285714</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <f aca="false">IF(D8&gt;0, E8/D8, 0)</f>
         <v>1.62790697674419</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <f aca="false">2/20*B9</f>
         <v>0.1</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="n">
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="n">
         <f aca="false">IF(D9&gt;0, E9/D9, 0)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="n">
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="n">
         <f aca="false">7.23*B10/1000</f>
         <v>0.11568</v>
       </c>
-      <c r="E10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="n">
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="n">
         <f aca="false">IF(D10&gt;0, E10/D10, 0)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="0" t="s">
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="n">
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="n">
         <f aca="false">11*B11/1000</f>
         <v>0.044</v>
       </c>
-      <c r="E11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="n">
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="n">
         <f aca="false">IF(D11&gt;0, E11/D11, 0)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="G11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D12" s="10" t="n">
+      <c r="D12" s="11" t="n">
         <f aca="false">SUM(D2:D11)</f>
         <v>6.5753581184669</v>
       </c>
-      <c r="E12" s="11" t="n">
+      <c r="E12" s="12" t="n">
         <f aca="false">SUM(E2:E11)</f>
         <v>27</v>
       </c>
-      <c r="F12" s="10" t="n">
+      <c r="F12" s="11" t="n">
         <f aca="false">IF(D12&gt;0, E12/D12, 0)</f>
         <v>4.10624022502599</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
     </row>
     <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1760,294 +1764,294 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="55.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="5.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.81"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <f aca="false">1.99/0.5*B2/1000</f>
         <v>0.5572</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <f aca="false">IF(D2&gt;0, E2/D2, 0)</f>
         <v>7.17875089734386</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="n">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <f aca="false">17.9*B3/1000</f>
         <v>0.0716</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <f aca="false">IF(D3&gt;0, E3/D3, 0)</f>
         <v>13.9664804469274</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <f aca="false">7.23*B4/1000</f>
         <v>0.11568</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <f aca="false">IF(D4&gt;0, E4/D4, 0)</f>
         <v>8.64453665283541</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>800</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="n">
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <f aca="false">(4+0.5)/2.46*B5/1000</f>
         <v>1.46341463414634</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="n">
+      <c r="E5" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4" t="n">
         <f aca="false">IF(D5&gt;0, E5/D5, 0)</f>
         <v>6.15</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="n">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <f aca="false">2.19/0.5*B6/1000</f>
         <v>2.19</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3" t="n">
+      <c r="E6" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="n">
         <f aca="false">IF(D6&gt;0, E6/D6, 0)</f>
         <v>4.5662100456621</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="n">
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <f aca="false">1.29/0.7*B7/1000</f>
         <v>1.84285714285714</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <f aca="false">IF(D7&gt;0, E7/D7, 0)</f>
         <v>2.17054263565891</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <f aca="false">2/20*B8</f>
         <v>0.1</v>
       </c>
-      <c r="E8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="n">
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="n">
         <f aca="false">IF(D8&gt;0, E8/D8, 0)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3" t="n">
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4" t="n">
         <f aca="false">20.99*B9/1000</f>
         <v>0.08396</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="n">
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="n">
         <f aca="false">IF(D9&gt;0, E9/D9, 0)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="0" t="s">
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="n">
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="n">
         <f aca="false">11*B10/1000</f>
         <v>0.044</v>
       </c>
-      <c r="E10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="n">
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="n">
         <f aca="false">IF(D10&gt;0, E10/D10, 0)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="0" t="s">
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="10" t="n">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11" t="n">
         <f aca="false">SUM(D2:D10)</f>
         <v>6.46871177700348</v>
       </c>
-      <c r="E11" s="11" t="n">
+      <c r="E11" s="12" t="n">
         <f aca="false">SUM(E2:E10)</f>
         <v>29</v>
       </c>
-      <c r="F11" s="10" t="n">
+      <c r="F11" s="11" t="n">
         <f aca="false">IF(D11&gt;0, E11/D11, 0)</f>
         <v>4.48311827759835</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F12" s="12"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2082,212 +2086,212 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="5.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.39"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <f aca="false">1.99/0.5*B2/1000</f>
         <v>0.5572</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <f aca="false">IF(D2&gt;0, E2/D2, 0)</f>
         <v>8.97343862167983</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="n">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <f aca="false">17.9*B3/1000</f>
         <v>0.2864</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <f aca="false">IF(D3&gt;0, E3/D3, 0)</f>
         <v>6.98324022346369</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>800</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <f aca="false">(4+0.5)/2.46*B4/1000</f>
         <v>1.46341463414634</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3" t="n">
+      <c r="E4" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="n">
         <f aca="false">IF(D4&gt;0, E4/D4, 0)</f>
         <v>6.83333333333333</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="n">
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <f aca="false">2.19/0.5*B5/1000</f>
         <v>2.19</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="n">
+      <c r="E5" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4" t="n">
         <f aca="false">IF(D5&gt;0, E5/D5, 0)</f>
         <v>4.10958904109589</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="n">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <f aca="false">1.29/0.7*B6/1000</f>
         <v>1.84285714285714</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <f aca="false">IF(D6&gt;0, E6/D6, 0)</f>
         <v>2.71317829457364</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <f aca="false">2/20*B7</f>
         <v>0.1</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="n">
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <f aca="false">IF(D7&gt;0, E7/D7, 0)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="10" t="n">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="11" t="n">
         <f aca="false">SUM(D2:D7)</f>
         <v>6.43987177700348</v>
       </c>
-      <c r="E8" s="11" t="n">
+      <c r="E8" s="12" t="n">
         <f aca="false">SUM(E2:E7)</f>
         <v>31</v>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="F8" s="11" t="n">
         <f aca="false">IF(D8&gt;0, E8/D8, 0)</f>
         <v>4.8137604401845</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F9" s="12"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F10" s="12"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2322,157 +2326,157 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="6.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="6.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+    <row r="1" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="13" t="n">
+      <c r="B2" s="14" t="n">
         <v>45989</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <f aca="false">1.15+0.05</f>
         <v>1.2</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="13" t="n">
+      <c r="F2" s="14" t="n">
         <v>46012</v>
       </c>
-      <c r="G2" s="14" t="n">
+      <c r="G2" s="15" t="n">
         <f aca="false">Fase1!D$15</f>
         <v>8.65473581881533</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="13" t="n">
+      <c r="B3" s="14" t="n">
         <f aca="false">F2+1</f>
         <v>46013</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <f aca="false">29+11</f>
         <v>40</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="13" t="n">
+      <c r="F3" s="14" t="n">
         <f aca="false">"3/12/2025"+D3/(12/7)</f>
         <v>46017.3333333333</v>
       </c>
-      <c r="G3" s="14" t="n">
+      <c r="G3" s="15" t="n">
         <f aca="false">Fase2!D$13</f>
-        <v>8.01525637630662</v>
+        <v>7.92311351916377</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="13" t="n">
+      <c r="B4" s="14" t="n">
         <f aca="false">F3+1</f>
         <v>46018.3333333333</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="13" t="n">
+      <c r="F4" s="14" t="n">
         <f aca="false">"4/12/2025"+D4/0.25</f>
         <v>46019</v>
       </c>
-      <c r="G4" s="14" t="n">
+      <c r="G4" s="15" t="n">
         <f aca="false">Fase3!D12</f>
         <v>6.5753581184669</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="14" t="n">
         <f aca="false">F4+1</f>
         <v>46020</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>0.6</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F5" s="14" t="n">
         <f aca="false">"4/12/2025"+D5/0.02</f>
         <v>46025</v>
       </c>
-      <c r="G5" s="14" t="n">
+      <c r="G5" s="15" t="n">
         <f aca="false">Fase4!D11</f>
         <v>6.46871177700348</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="13" t="n">
+      <c r="B6" s="14" t="n">
         <f aca="false">F5+1</f>
         <v>46026</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="13" t="n">
+      <c r="F6" s="14" t="n">
         <v>47483</v>
       </c>
-      <c r="G6" s="14" t="n">
+      <c r="G6" s="15" t="n">
         <f aca="false">Fase5!D8</f>
         <v>6.43987177700348</v>
       </c>

</xml_diff>